<commit_message>
Updated and harmonized controlled vocabs for Templates for 2021Q4
</commit_message>
<xml_diff>
--- a/Templates/sample_inventory/Sample_Inventory_Metadata_2021Q4_template.xlsx
+++ b/Templates/sample_inventory/Sample_Inventory_Metadata_2021Q4_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pam.baker/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pam.baker/Documents/repos/BCDC-Metadata/Templates/sample_inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06228155-D852-2345-A051-916E2638FF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AEC6B8-00BE-734F-81B8-49F03B4E27D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26400" windowHeight="17220" tabRatio="599" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8080" yWindow="460" windowWidth="23620" windowHeight="17220" tabRatio="599" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="READ_ME" sheetId="3" r:id="rId1"/>
@@ -19,10 +19,9 @@
     <sheet name="Data_Collections_CV" sheetId="11" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Controlled Values'!$C$3:$C$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Controlled Values'!$C$3:$C$16</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="812">
   <si>
     <t>Sample Level Metadata:</t>
   </si>
@@ -2480,6 +2479,21 @@
   </si>
   <si>
     <t>Changes to template for December 2021</t>
+  </si>
+  <si>
+    <t>anatomy</t>
+  </si>
+  <si>
+    <t>electrophysiology</t>
+  </si>
+  <si>
+    <t>genomics</t>
+  </si>
+  <si>
+    <t>histology imaging</t>
+  </si>
+  <si>
+    <t>optical physiology</t>
   </si>
 </sst>
 </file>
@@ -4511,8 +4525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S74"/>
   <sheetViews>
-    <sheetView topLeftCell="F10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4623,8 +4637,8 @@
         <v>74</v>
       </c>
       <c r="B4" s="26"/>
-      <c r="C4" s="18" t="s">
-        <v>75</v>
+      <c r="C4" s="36" t="s">
+        <v>807</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="48" t="s">
@@ -4661,7 +4675,7 @@
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="18" t="s">
@@ -4700,7 +4714,7 @@
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="18" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="18" t="s">
@@ -4736,7 +4750,7 @@
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="18" t="s">
-        <v>100</v>
+        <v>808</v>
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="18" t="s">
@@ -4768,7 +4782,7 @@
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="18" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D8" s="26"/>
       <c r="E8" s="18" t="s">
@@ -4802,7 +4816,7 @@
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="18" t="s">
-        <v>113</v>
+        <v>809</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="18" t="s">
@@ -4836,7 +4850,7 @@
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="18" t="s">
-        <v>120</v>
+        <v>810</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="18" t="s">
@@ -4862,13 +4876,13 @@
       <c r="R10" s="26"/>
       <c r="S10" s="26"/>
     </row>
-    <row r="11" spans="1:19" ht="16" thickBot="1">
+    <row r="11" spans="1:19">
       <c r="A11" s="41" t="s">
         <v>125</v>
       </c>
       <c r="B11" s="26"/>
-      <c r="C11" s="19" t="s">
-        <v>126</v>
+      <c r="C11" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="18" t="s">
@@ -4901,7 +4915,9 @@
         <v>132</v>
       </c>
       <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
+      <c r="C12" s="18" t="s">
+        <v>811</v>
+      </c>
       <c r="D12" s="26"/>
       <c r="E12" s="18" t="s">
         <v>114</v>
@@ -4933,7 +4949,9 @@
         <v>138</v>
       </c>
       <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+      <c r="C13" s="18" t="s">
+        <v>106</v>
+      </c>
       <c r="D13" s="26"/>
       <c r="E13" s="18" t="s">
         <v>121</v>
@@ -4963,7 +4981,9 @@
         <v>143</v>
       </c>
       <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
+      <c r="C14" s="18" t="s">
+        <v>113</v>
+      </c>
       <c r="D14" s="26"/>
       <c r="E14" s="18" t="s">
         <v>601</v>
@@ -4995,7 +5015,9 @@
         <v>149</v>
       </c>
       <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
+      <c r="C15" s="18" t="s">
+        <v>120</v>
+      </c>
       <c r="D15" s="26"/>
       <c r="E15" s="18" t="s">
         <v>127</v>
@@ -5022,12 +5044,14 @@
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" ht="16" thickBot="1">
       <c r="A16" s="41" t="s">
         <v>155</v>
       </c>
       <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
+      <c r="C16" s="19" t="s">
+        <v>126</v>
+      </c>
       <c r="D16" s="26"/>
       <c r="E16" s="18" t="s">
         <v>602</v>
@@ -5916,9 +5940,7 @@
         <v>222</v>
       </c>
       <c r="B52" s="16"/>
-      <c r="C52" s="16" t="s">
-        <v>222</v>
-      </c>
+      <c r="C52" s="26"/>
       <c r="D52" s="47"/>
       <c r="E52" s="16" t="s">
         <v>222</v>
@@ -5938,9 +5960,7 @@
         <v>225</v>
       </c>
       <c r="B53" s="26"/>
-      <c r="C53" s="26" t="s">
-        <v>225</v>
-      </c>
+      <c r="C53" s="26"/>
       <c r="E53" s="26" t="s">
         <v>225</v>
       </c>
@@ -5958,9 +5978,7 @@
         <v>227</v>
       </c>
       <c r="B54" s="26"/>
-      <c r="C54" s="26" t="s">
-        <v>227</v>
-      </c>
+      <c r="C54" s="26"/>
       <c r="E54" s="26" t="s">
         <v>227</v>
       </c>
@@ -5978,9 +5996,7 @@
         <v>235</v>
       </c>
       <c r="B55" s="26"/>
-      <c r="C55" s="26" t="s">
-        <v>229</v>
-      </c>
+      <c r="C55" s="26"/>
       <c r="E55" s="26" t="s">
         <v>229</v>
       </c>
@@ -5996,9 +6012,7 @@
     <row r="56" spans="1:16">
       <c r="A56" s="26"/>
       <c r="B56" s="26"/>
-      <c r="C56" s="26" t="s">
-        <v>238</v>
-      </c>
+      <c r="C56" s="26"/>
       <c r="E56" s="26" t="s">
         <v>232</v>
       </c>
@@ -6014,7 +6028,9 @@
     <row r="57" spans="1:16">
       <c r="A57" s="26"/>
       <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
+      <c r="C57" s="16" t="s">
+        <v>222</v>
+      </c>
       <c r="E57" t="s">
         <v>619</v>
       </c>
@@ -6030,7 +6046,9 @@
     <row r="58" spans="1:16">
       <c r="A58" s="26"/>
       <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
+      <c r="C58" s="26" t="s">
+        <v>225</v>
+      </c>
       <c r="I58" s="26"/>
       <c r="J58" s="26"/>
       <c r="K58" s="26"/>
@@ -6041,6 +6059,9 @@
       <c r="P58" s="26"/>
     </row>
     <row r="59" spans="1:16">
+      <c r="C59" s="26" t="s">
+        <v>227</v>
+      </c>
       <c r="I59" s="26"/>
       <c r="J59" s="26"/>
       <c r="K59" s="26"/>
@@ -6051,6 +6072,9 @@
       <c r="P59" s="26"/>
     </row>
     <row r="60" spans="1:16">
+      <c r="C60" s="26" t="s">
+        <v>229</v>
+      </c>
       <c r="I60" s="26"/>
       <c r="J60" s="26"/>
       <c r="K60" s="26"/>
@@ -6061,6 +6085,9 @@
       <c r="P60" s="26"/>
     </row>
     <row r="61" spans="1:16">
+      <c r="C61" s="26" t="s">
+        <v>238</v>
+      </c>
       <c r="I61" s="26"/>
       <c r="J61" s="26"/>
       <c r="K61" s="26"/>
@@ -6071,6 +6098,7 @@
       <c r="P61" s="26"/>
     </row>
     <row r="62" spans="1:16">
+      <c r="C62" s="26"/>
       <c r="I62" s="26"/>
       <c r="J62" s="26"/>
       <c r="K62" s="26"/>
@@ -6081,6 +6109,7 @@
       <c r="P62" s="26"/>
     </row>
     <row r="63" spans="1:16">
+      <c r="C63" s="26"/>
       <c r="I63" s="26"/>
       <c r="J63" s="26"/>
       <c r="K63" s="26"/>
@@ -6169,7 +6198,7 @@
       <c r="J74" s="26"/>
     </row>
   </sheetData>
-  <autoFilter ref="C3:C11" xr:uid="{6D307B3E-6034-4F21-9567-189C6482E023}"/>
+  <autoFilter ref="C3:C16" xr:uid="{6D307B3E-6034-4F21-9567-189C6482E023}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K4:K28">
     <sortCondition ref="K4"/>
   </sortState>
@@ -6185,7 +6214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EDC583-1A24-4950-A0DA-611E0CF11932}">
   <dimension ref="A1:G289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
@@ -10009,12 +10038,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="0af18bdd-3447-408d-80d3-6f9fce434a6a" xsi:nil="true"/>
+    <SharedWithUsers xmlns="ce57bbcd-944d-48da-b7d9-79b20bf66928">
+      <UserInfo>
+        <DisplayName>Tim Fliss</DisplayName>
+        <AccountId>767</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10249,24 +10284,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="0af18bdd-3447-408d-80d3-6f9fce434a6a" xsi:nil="true"/>
-    <SharedWithUsers xmlns="ce57bbcd-944d-48da-b7d9-79b20bf66928">
-      <UserInfo>
-        <DisplayName>Tim Fliss</DisplayName>
-        <AccountId>767</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77F7C331-08C4-4F14-8B6A-29CD8DF47E6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8494D3F1-3EF7-4062-8C18-CF37BCAAC176}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0af18bdd-3447-408d-80d3-6f9fce434a6a"/>
+    <ds:schemaRef ds:uri="ce57bbcd-944d-48da-b7d9-79b20bf66928"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10291,12 +10323,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8494D3F1-3EF7-4062-8C18-CF37BCAAC176}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77F7C331-08C4-4F14-8B6A-29CD8DF47E6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0af18bdd-3447-408d-80d3-6f9fce434a6a"/>
-    <ds:schemaRef ds:uri="ce57bbcd-944d-48da-b7d9-79b20bf66928"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated and harmonized controlled vocabs for Templates for 2021Q4 (#29)
Co-authored-by: Pam Baker <pamela.baker@alleninstitute.org>
</commit_message>
<xml_diff>
--- a/Templates/sample_inventory/Sample_Inventory_Metadata_2021Q4_template.xlsx
+++ b/Templates/sample_inventory/Sample_Inventory_Metadata_2021Q4_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pam.baker/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pam.baker/Documents/repos/BCDC-Metadata/Templates/sample_inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06228155-D852-2345-A051-916E2638FF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AEC6B8-00BE-734F-81B8-49F03B4E27D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26400" windowHeight="17220" tabRatio="599" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8080" yWindow="460" windowWidth="23620" windowHeight="17220" tabRatio="599" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="READ_ME" sheetId="3" r:id="rId1"/>
@@ -19,10 +19,9 @@
     <sheet name="Data_Collections_CV" sheetId="11" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Controlled Values'!$C$3:$C$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Controlled Values'!$C$3:$C$16</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="812">
   <si>
     <t>Sample Level Metadata:</t>
   </si>
@@ -2480,6 +2479,21 @@
   </si>
   <si>
     <t>Changes to template for December 2021</t>
+  </si>
+  <si>
+    <t>anatomy</t>
+  </si>
+  <si>
+    <t>electrophysiology</t>
+  </si>
+  <si>
+    <t>genomics</t>
+  </si>
+  <si>
+    <t>histology imaging</t>
+  </si>
+  <si>
+    <t>optical physiology</t>
   </si>
 </sst>
 </file>
@@ -4511,8 +4525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S74"/>
   <sheetViews>
-    <sheetView topLeftCell="F10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4623,8 +4637,8 @@
         <v>74</v>
       </c>
       <c r="B4" s="26"/>
-      <c r="C4" s="18" t="s">
-        <v>75</v>
+      <c r="C4" s="36" t="s">
+        <v>807</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="48" t="s">
@@ -4661,7 +4675,7 @@
       </c>
       <c r="B5" s="26"/>
       <c r="C5" s="18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="18" t="s">
@@ -4700,7 +4714,7 @@
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="18" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="18" t="s">
@@ -4736,7 +4750,7 @@
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="18" t="s">
-        <v>100</v>
+        <v>808</v>
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="18" t="s">
@@ -4768,7 +4782,7 @@
       </c>
       <c r="B8" s="26"/>
       <c r="C8" s="18" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="D8" s="26"/>
       <c r="E8" s="18" t="s">
@@ -4802,7 +4816,7 @@
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="18" t="s">
-        <v>113</v>
+        <v>809</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="18" t="s">
@@ -4836,7 +4850,7 @@
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="18" t="s">
-        <v>120</v>
+        <v>810</v>
       </c>
       <c r="D10" s="26"/>
       <c r="E10" s="18" t="s">
@@ -4862,13 +4876,13 @@
       <c r="R10" s="26"/>
       <c r="S10" s="26"/>
     </row>
-    <row r="11" spans="1:19" ht="16" thickBot="1">
+    <row r="11" spans="1:19">
       <c r="A11" s="41" t="s">
         <v>125</v>
       </c>
       <c r="B11" s="26"/>
-      <c r="C11" s="19" t="s">
-        <v>126</v>
+      <c r="C11" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="D11" s="26"/>
       <c r="E11" s="18" t="s">
@@ -4901,7 +4915,9 @@
         <v>132</v>
       </c>
       <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
+      <c r="C12" s="18" t="s">
+        <v>811</v>
+      </c>
       <c r="D12" s="26"/>
       <c r="E12" s="18" t="s">
         <v>114</v>
@@ -4933,7 +4949,9 @@
         <v>138</v>
       </c>
       <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
+      <c r="C13" s="18" t="s">
+        <v>106</v>
+      </c>
       <c r="D13" s="26"/>
       <c r="E13" s="18" t="s">
         <v>121</v>
@@ -4963,7 +4981,9 @@
         <v>143</v>
       </c>
       <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
+      <c r="C14" s="18" t="s">
+        <v>113</v>
+      </c>
       <c r="D14" s="26"/>
       <c r="E14" s="18" t="s">
         <v>601</v>
@@ -4995,7 +5015,9 @@
         <v>149</v>
       </c>
       <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
+      <c r="C15" s="18" t="s">
+        <v>120</v>
+      </c>
       <c r="D15" s="26"/>
       <c r="E15" s="18" t="s">
         <v>127</v>
@@ -5022,12 +5044,14 @@
       <c r="R15" s="26"/>
       <c r="S15" s="26"/>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" ht="16" thickBot="1">
       <c r="A16" s="41" t="s">
         <v>155</v>
       </c>
       <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
+      <c r="C16" s="19" t="s">
+        <v>126</v>
+      </c>
       <c r="D16" s="26"/>
       <c r="E16" s="18" t="s">
         <v>602</v>
@@ -5916,9 +5940,7 @@
         <v>222</v>
       </c>
       <c r="B52" s="16"/>
-      <c r="C52" s="16" t="s">
-        <v>222</v>
-      </c>
+      <c r="C52" s="26"/>
       <c r="D52" s="47"/>
       <c r="E52" s="16" t="s">
         <v>222</v>
@@ -5938,9 +5960,7 @@
         <v>225</v>
       </c>
       <c r="B53" s="26"/>
-      <c r="C53" s="26" t="s">
-        <v>225</v>
-      </c>
+      <c r="C53" s="26"/>
       <c r="E53" s="26" t="s">
         <v>225</v>
       </c>
@@ -5958,9 +5978,7 @@
         <v>227</v>
       </c>
       <c r="B54" s="26"/>
-      <c r="C54" s="26" t="s">
-        <v>227</v>
-      </c>
+      <c r="C54" s="26"/>
       <c r="E54" s="26" t="s">
         <v>227</v>
       </c>
@@ -5978,9 +5996,7 @@
         <v>235</v>
       </c>
       <c r="B55" s="26"/>
-      <c r="C55" s="26" t="s">
-        <v>229</v>
-      </c>
+      <c r="C55" s="26"/>
       <c r="E55" s="26" t="s">
         <v>229</v>
       </c>
@@ -5996,9 +6012,7 @@
     <row r="56" spans="1:16">
       <c r="A56" s="26"/>
       <c r="B56" s="26"/>
-      <c r="C56" s="26" t="s">
-        <v>238</v>
-      </c>
+      <c r="C56" s="26"/>
       <c r="E56" s="26" t="s">
         <v>232</v>
       </c>
@@ -6014,7 +6028,9 @@
     <row r="57" spans="1:16">
       <c r="A57" s="26"/>
       <c r="B57" s="26"/>
-      <c r="C57" s="26"/>
+      <c r="C57" s="16" t="s">
+        <v>222</v>
+      </c>
       <c r="E57" t="s">
         <v>619</v>
       </c>
@@ -6030,7 +6046,9 @@
     <row r="58" spans="1:16">
       <c r="A58" s="26"/>
       <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
+      <c r="C58" s="26" t="s">
+        <v>225</v>
+      </c>
       <c r="I58" s="26"/>
       <c r="J58" s="26"/>
       <c r="K58" s="26"/>
@@ -6041,6 +6059,9 @@
       <c r="P58" s="26"/>
     </row>
     <row r="59" spans="1:16">
+      <c r="C59" s="26" t="s">
+        <v>227</v>
+      </c>
       <c r="I59" s="26"/>
       <c r="J59" s="26"/>
       <c r="K59" s="26"/>
@@ -6051,6 +6072,9 @@
       <c r="P59" s="26"/>
     </row>
     <row r="60" spans="1:16">
+      <c r="C60" s="26" t="s">
+        <v>229</v>
+      </c>
       <c r="I60" s="26"/>
       <c r="J60" s="26"/>
       <c r="K60" s="26"/>
@@ -6061,6 +6085,9 @@
       <c r="P60" s="26"/>
     </row>
     <row r="61" spans="1:16">
+      <c r="C61" s="26" t="s">
+        <v>238</v>
+      </c>
       <c r="I61" s="26"/>
       <c r="J61" s="26"/>
       <c r="K61" s="26"/>
@@ -6071,6 +6098,7 @@
       <c r="P61" s="26"/>
     </row>
     <row r="62" spans="1:16">
+      <c r="C62" s="26"/>
       <c r="I62" s="26"/>
       <c r="J62" s="26"/>
       <c r="K62" s="26"/>
@@ -6081,6 +6109,7 @@
       <c r="P62" s="26"/>
     </row>
     <row r="63" spans="1:16">
+      <c r="C63" s="26"/>
       <c r="I63" s="26"/>
       <c r="J63" s="26"/>
       <c r="K63" s="26"/>
@@ -6169,7 +6198,7 @@
       <c r="J74" s="26"/>
     </row>
   </sheetData>
-  <autoFilter ref="C3:C11" xr:uid="{6D307B3E-6034-4F21-9567-189C6482E023}"/>
+  <autoFilter ref="C3:C16" xr:uid="{6D307B3E-6034-4F21-9567-189C6482E023}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K4:K28">
     <sortCondition ref="K4"/>
   </sortState>
@@ -6185,7 +6214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6EDC583-1A24-4950-A0DA-611E0CF11932}">
   <dimension ref="A1:G289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
@@ -10009,12 +10038,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="0af18bdd-3447-408d-80d3-6f9fce434a6a" xsi:nil="true"/>
+    <SharedWithUsers xmlns="ce57bbcd-944d-48da-b7d9-79b20bf66928">
+      <UserInfo>
+        <DisplayName>Tim Fliss</DisplayName>
+        <AccountId>767</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10249,24 +10284,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="0af18bdd-3447-408d-80d3-6f9fce434a6a" xsi:nil="true"/>
-    <SharedWithUsers xmlns="ce57bbcd-944d-48da-b7d9-79b20bf66928">
-      <UserInfo>
-        <DisplayName>Tim Fliss</DisplayName>
-        <AccountId>767</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77F7C331-08C4-4F14-8B6A-29CD8DF47E6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8494D3F1-3EF7-4062-8C18-CF37BCAAC176}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0af18bdd-3447-408d-80d3-6f9fce434a6a"/>
+    <ds:schemaRef ds:uri="ce57bbcd-944d-48da-b7d9-79b20bf66928"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10291,12 +10323,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8494D3F1-3EF7-4062-8C18-CF37BCAAC176}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{77F7C331-08C4-4F14-8B6A-29CD8DF47E6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0af18bdd-3447-408d-80d3-6f9fce434a6a"/>
-    <ds:schemaRef ds:uri="ce57bbcd-944d-48da-b7d9-79b20bf66928"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>